<commit_message>
Thống kê tiêm phòng
</commit_message>
<xml_diff>
--- a/assets/excel/MauImportVaccine.xlsx
+++ b/assets/excel/MauImportVaccine.xlsx
@@ -9,8 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Tên chủ hộ</t>
   </si>
@@ -46,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Giống</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày sinh</t>
   </si>
   <si>
     <t xml:space="preserve">Ngày tiêm</t>
@@ -154,24 +155,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.05"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="15.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -201,6 +193,9 @@
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -212,50 +207,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
thêm dropbox cho phường
</commit_message>
<xml_diff>
--- a/assets/excel/MauImportVaccine.xlsx
+++ b/assets/excel/MauImportVaccine.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="danh sách phường" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Tên chủ hộ</t>
   </si>
@@ -53,6 +54,72 @@
   </si>
   <si>
     <t xml:space="preserve">Ngày tiêm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Lộc Thọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Ngọc Hiệp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Phước Hải</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Phước Hòa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Phước Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Phước Tân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Phương Sài</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Phương Sơn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Tân Lập</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường vạn Thắng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Vạn Thạnh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Vĩnh Hải</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Vĩnh Hòa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Vĩnh Nguyên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Vĩnh Phước</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Vĩnh Trường</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phường Xương Huân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xã Vĩnh Hiệp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xã Vĩnh Lương</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xã Vĩnh Ngọc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xã Vĩnh Phương</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xã Vĩnh Thạnh</t>
   </si>
 </sst>
 </file>
@@ -129,13 +196,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -158,7 +233,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -202,10 +277,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D1001" type="list">
+      <formula1>'danh sách phường'!$A$1:$A$22</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -214,4 +295,141 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.32"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>